<commit_message>
Populate the new template with existing distinct labels
</commit_message>
<xml_diff>
--- a/uploads/allPages.xlsx
+++ b/uploads/allPages.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Label_name</t>
   </si>
@@ -21,6 +21,57 @@
   </si>
   <si>
     <t>Language_id</t>
+  </si>
+  <si>
+    <t>userDatabase</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>newLanguage</t>
+  </si>
+  <si>
+    <t>newPage</t>
+  </si>
+  <si>
+    <t>newLabel</t>
+  </si>
+  <si>
+    <t>updateLabel</t>
+  </si>
+  <si>
+    <t>fullTemplate</t>
+  </si>
+  <si>
+    <t>downloadTemplates</t>
+  </si>
+  <si>
+    <t>completeUpload</t>
+  </si>
+  <si>
+    <t>signUp</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -408,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="28" customWidth="1"/>
@@ -425,15 +476,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1-US-en,2-IN-hi,3-IN-kn,4-es,5-EU-Ge,6-EU-fr"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1-US-en,2-IN-hi,3-IN-kn,4-es,5-EU-Ge,6-EU-fr"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
@@ -441,7 +534,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="28" customWidth="1"/>
@@ -458,15 +551,47 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1-US-en,2-IN-hi,3-IN-kn,4-es,5-EU-Ge,6-EU-fr"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1-US-en,2-IN-hi,3-IN-kn,4-es,5-EU-Ge,6-EU-fr"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added extra fields for translation in dashboard page
</commit_message>
<xml_diff>
--- a/uploads/allPages.xlsx
+++ b/uploads/allPages.xlsx
@@ -527,6 +527,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
@@ -592,6 +600,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes after new branch
</commit_message>
<xml_diff>
--- a/uploads/allPages.xlsx
+++ b/uploads/allPages.xlsx
@@ -6,13 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="1 dashboard" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="2 signup" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="3 homePage" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Label_name</t>
   </si>
@@ -529,10 +530,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -602,10 +603,43 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="C10:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C500">
-      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr"</formula1>
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="C10:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C500">
+      <formula1>"1 US-en,2 IN-hi,3 IN-kn,4 es,5 EU-Ge,6 EU-fr,7 Chinese,8 Russian"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>